<commit_message>
fixed "random sound piece" slot and player on views
</commit_message>
<xml_diff>
--- a/scheduleSheet/schedule.xlsx
+++ b/scheduleSheet/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\X\Developer\imca-raydeeoh\schedule\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/SWOON1/Documents/GitHub/imca-raydeeoh/scheduleSheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D82DFD0D-2691-40E4-89D0-C067E3FC301D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C1DC9B-FBBB-8E48-B8BD-BA4365628098}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16560" yWindow="0" windowWidth="21820" windowHeight="15780" xr2:uid="{C1F8DBFD-48D2-814D-8C9A-C834504E829D}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" xr2:uid="{C1F8DBFD-48D2-814D-8C9A-C834504E829D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="74">
   <si>
     <t>Day</t>
   </si>
@@ -174,9 +174,6 @@
     <t>Mc.pale</t>
   </si>
   <si>
-    <t>DIRTY STINKY SMELLY</t>
-  </si>
-  <si>
     <t>Within a matter of seconds, my pitch shifted voice flangs into what feels like 'Search History' you thought you had cleared, we descend into the seductive, the surreal, the "DIRTY STINKY SMELLY". It is a variety show lathered with provocations – cleaning up all that nasty noise by dumping its proverbial garbage basket all over your desk and lighting it on fire. Think reality television play-by-plays shows, 5 gum, DIY night-core, sexy whistling, clock-ticking, clown costumes... It is a show that places horrible content right beneath our noses in the form of experimental sound, "trash" pop-culture indulgence and live prop-comedy performance.</t>
   </si>
   <si>
@@ -256,6 +253,12 @@
   </si>
   <si>
     <t>SPINCYCLES [replay]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PWUPPY PWINCESS </t>
+  </si>
+  <si>
+    <t>DIRTY STINKY SMELLY (…)</t>
   </si>
 </sst>
 </file>
@@ -263,7 +266,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -336,11 +339,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="6" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -349,6 +352,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -667,18 +673,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{509B4220-E834-8A48-82FB-A9FB9AAA8E06}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="53.6640625" customWidth="1"/>
     <col min="3" max="3" width="26.6640625" customWidth="1"/>
     <col min="4" max="4" width="71.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -695,7 +701,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -712,7 +718,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -729,7 +735,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -746,7 +752,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -763,7 +769,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -780,7 +786,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -797,12 +803,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" t="s">
         <v>25</v>
@@ -814,7 +820,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -831,10 +837,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" s="10"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>4</v>
       </c>
@@ -851,7 +857,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
@@ -868,7 +874,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -885,7 +891,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>4</v>
       </c>
@@ -902,66 +908,66 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>45</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>46</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>45</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>46</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B17" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>48</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>49</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B18" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>36</v>
@@ -970,10 +976,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B19" s="10"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -990,29 +996,29 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>5</v>
       </c>
       <c r="B21" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="D21" s="8" t="s">
         <v>53</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>54</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>5</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C22" t="s">
         <v>25</v>
@@ -1024,7 +1030,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -1041,63 +1047,63 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>5</v>
       </c>
       <c r="B24" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" t="s">
         <v>57</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" s="8" t="s">
         <v>58</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>59</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>5</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>5</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>5</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C27" t="s">
         <v>22</v>
@@ -1109,15 +1115,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B28" s="10"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C29" t="s">
         <v>31</v>
@@ -1129,15 +1135,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>36</v>
@@ -1146,12 +1152,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C31" t="s">
         <v>32</v>
@@ -1163,7 +1169,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>6</v>
       </c>
@@ -1180,12 +1186,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>44</v>
@@ -1197,7 +1203,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>6</v>
       </c>
@@ -1214,12 +1220,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>41</v>
@@ -1231,12 +1237,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C36" t="s">
         <v>30</v>
@@ -1248,28 +1254,28 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B37" s="10"/>
       <c r="E37" s="1"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C38" t="s">
+        <v>57</v>
+      </c>
+      <c r="D38" s="8" t="s">
         <v>58</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>59</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>7</v>
       </c>
@@ -1286,7 +1292,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>7</v>
       </c>
@@ -1303,7 +1309,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>7</v>
       </c>
@@ -1320,75 +1326,75 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C42" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D42" s="8" t="s">
         <v>48</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>49</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C45" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D45" s="8" t="s">
         <v>53</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>54</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E46" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
schedule is complete (--:
</commit_message>
<xml_diff>
--- a/scheduleSheet/schedule.xlsx
+++ b/scheduleSheet/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/SWOON1/Documents/GitHub/imca-raydeeoh/scheduleSheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47478145-9B59-F94A-A3BC-3C11F96096CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2DE2C71-718F-5148-9D9C-5FD6D3F47335}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14080" xr2:uid="{C1F8DBFD-48D2-814D-8C9A-C834504E829D}"/>
   </bookViews>
@@ -147,9 +147,6 @@
     <t>Esotalk</t>
   </si>
   <si>
-    <t>??</t>
-  </si>
-  <si>
     <t>☆</t>
   </si>
   <si>
@@ -244,6 +241,9 @@
   </si>
   <si>
     <t>This recording is made using a Pure Data patch that requests a file of solar wind measurements from the ACE satellite (http://www.srl.caltech.edu/ACE/) every two minutes. The North-South magnetic field intensity from the past two hours is played back over two minutes as notes in a 17-tone scale. The sound is Karplus-Strong string synthesis made to emulate a bowed instrument. The sound is then passed through a delay with feedback, whose length changes according to the magnetic field intensity.</t>
+  </si>
+  <si>
+    <t>Two 30-minute soundscapes by two babies from the Maritimes, trying to catch some relaxing vibes in the city</t>
   </si>
 </sst>
 </file>
@@ -703,7 +703,7 @@
   <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -787,13 +787,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s">
         <v>40</v>
       </c>
-      <c r="C6" t="s">
-        <v>41</v>
-      </c>
       <c r="D6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>12</v>
@@ -804,13 +804,13 @@
         <v>3</v>
       </c>
       <c r="B7" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" t="s">
         <v>42</v>
       </c>
-      <c r="C7" t="s">
-        <v>43</v>
-      </c>
       <c r="D7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>13</v>
@@ -821,7 +821,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
         <v>21</v>
@@ -838,13 +838,13 @@
         <v>3</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>15</v>
@@ -910,13 +910,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>23</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>12</v>
@@ -927,13 +927,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>23</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>13</v>
@@ -944,13 +944,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C17" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="16" t="s">
         <v>56</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>57</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>14</v>
@@ -961,13 +961,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>15</v>
@@ -1036,7 +1036,7 @@
         <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>26</v>
@@ -1056,7 +1056,7 @@
         <v>28</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>13</v>
@@ -1067,13 +1067,13 @@
         <v>5</v>
       </c>
       <c r="B26" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="D26" s="8" t="s">
         <v>67</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>68</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>14</v>
@@ -1084,13 +1084,13 @@
         <v>5</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>15</v>
@@ -1156,10 +1156,10 @@
         <v>6</v>
       </c>
       <c r="B33" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>48</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>29</v>
@@ -1173,13 +1173,13 @@
         <v>6</v>
       </c>
       <c r="B34" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34" s="8" t="s">
         <v>64</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>65</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>13</v>
@@ -1190,13 +1190,13 @@
         <v>6</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>14</v>
@@ -1207,13 +1207,13 @@
         <v>6</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>15</v>
@@ -1303,7 +1303,7 @@
         <v>30</v>
       </c>
       <c r="D43" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>13</v>
@@ -1331,13 +1331,13 @@
         <v>7</v>
       </c>
       <c r="B45" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C45" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C45" s="7" t="s">
-        <v>63</v>
-      </c>
       <c r="D45" s="8" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
updated schedule for replay week!
</commit_message>
<xml_diff>
--- a/scheduleSheet/schedule.xlsx
+++ b/scheduleSheet/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/SWOON1/Documents/GitHub/imca-raydeeoh/scheduleSheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2DE2C71-718F-5148-9D9C-5FD6D3F47335}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8A209D-85C1-D64B-949F-24DFEAE3E2C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14080" xr2:uid="{C1F8DBFD-48D2-814D-8C9A-C834504E829D}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="69">
   <si>
     <t>Day</t>
   </si>
@@ -108,9 +108,6 @@
     <t>~~~</t>
   </si>
   <si>
-    <t>You Look Fine</t>
-  </si>
-  <si>
     <t xml:space="preserve">Using the structure of a talk-show/podcast, we would like to welcome different artists from across campus to share their experiences of being a creator living with chronic illness and or invisible disability. We are interested in how their illness(es) has influenced their practice and how they face the struggles they experience due to their illness(es) in and out of their practice. One part of the show would be a segment speaking about the illness(es) of the guest artist in order to raise awareness and offer helpful resources for those who might also be struggling with the same illness(es). Another segment would include an artist spotlight, giving each artist the opportunity to share one of their own art pieces/performances/creations. The overall goal of the show would be to raise visibility for the chronically ill &amp; invisibly disabled community on campus and hopefully create a community of artists who can collaborate and support one another. </t>
   </si>
   <si>
@@ -123,9 +120,6 @@
     <t>Within a matter of seconds, my pitch shifted voice flangs into what feels like 'Search History' you thought you had cleared, we descend into the seductive, the surreal, the "DIRTY STINKY SMELLY". It is a variety show lathered with provocations – cleaning up all that nasty noise by dumping its proverbial garbage basket all over your desk and lighting it on fire. Think reality television play-by-plays shows, 5 gum, DIY night-core, sexy whistling, clock-ticking, clown costumes... It is a show that places horrible content right beneath our noses in the form of experimental sound, "trash" pop-culture indulgence and live prop-comedy performance.</t>
   </si>
   <si>
-    <t>Hakeem Lapointe</t>
-  </si>
-  <si>
     <t>iced t</t>
   </si>
   <si>
@@ -135,9 +129,6 @@
     <t>offline</t>
   </si>
   <si>
-    <t>ADHD-Fueled Scattered Interests: Plunderphonics and John Oswald</t>
-  </si>
-  <si>
     <t>Postamateur</t>
   </si>
   <si>
@@ -156,9 +147,6 @@
     <t>Sara-Claudia Ligondé</t>
   </si>
   <si>
-    <t xml:space="preserve">Boioioing! </t>
-  </si>
-  <si>
     <t>Ale(OS)</t>
   </si>
   <si>
@@ -169,12 +157,6 @@
   </si>
   <si>
     <t>Lunam Theatre Company</t>
-  </si>
-  <si>
-    <t>DIRTY STINKY SMELLY […]</t>
-  </si>
-  <si>
-    <t>PWUPPY PWINCESS WITH SPECIAL GUEST DON'T TALK TO MY CLIENT EVER AGAIN</t>
   </si>
   <si>
     <t>Casual Fridays</t>
@@ -195,55 +177,71 @@
     <t xml:space="preserve">Midly amusing shit (M.A.S) serait une émission radio ou moi et divers collaborateurs parleraient de trucs sous le large thème de la culture. Sketch, critique, éditoriaux et chroniques seraient au menu. J’aimerais amener à l’université un regard qui ne se prend pas au sérieux quant à l’art et la culture, l’émission se veut humoristique et qui ose un peu des fois mais pas trop. </t>
   </si>
   <si>
-    <t>Live performance exploring time and space with a variety of synthesizers.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Presenting and explaining the work of John Oswald and Audio Piracy as a creative prerogative in an accessible way with audio. 20% talking 80% music : - ) </t>
   </si>
   <si>
-    <t xml:space="preserve">SAGE aka victor/Juice it Up! </t>
-  </si>
-  <si>
-    <t>Midly amusing shit (M.A.S) serait une émission radio ou moi et divers collaborateurs parleraient de trucs sous le large thème de la culture. Sketch, critique, éditoriaux et chroniques seraient au menu. J’aimerais amener à l’université un regard qui ne se prend pas au sérieux quant à l’art et la culture, l’émission se veut humoristique et qui ose un peu des fois mais pas trop. 
-/
-An interesting dichotomy of absurdist humor and experimental voices, we bet you will LOL a lot or be like "damn this shit is good!" 
+    <t>Though MANIC is a solo endeavour, this compilation features many collaborations; namely with Dave Ewenson, Solomon Vroman, Yaya Wagg, Jeremy Costello and Camella Lobo. Adverse to drawing influence through genre; these sonic explorations are as poetic in ethos as they are in content. Recorded 2010-2015.</t>
+  </si>
+  <si>
+    <t>MANIC</t>
+  </si>
+  <si>
+    <t>the ancient ruins of modernity</t>
+  </si>
+  <si>
+    <t>East Coast Lifestyle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compilation including the sounds of Casio CA-100, CTK-450, CT-657, CT-700, EP-20, MT-240, PT-88, SK-5, SK-1, SA-1, SA-7, SA-75 and the VL-1. </t>
+  </si>
+  <si>
+    <t>Solarise</t>
+  </si>
+  <si>
+    <t>Martin Peach</t>
+  </si>
+  <si>
+    <t>This recording is made using a Pure Data patch that requests a file of solar wind measurements from the ACE satellite (http://www.srl.caltech.edu/ACE/) every two minutes. The North-South magnetic field intensity from the past two hours is played back over two minutes as notes in a 17-tone scale. The sound is Karplus-Strong string synthesis made to emulate a bowed instrument. The sound is then passed through a delay with feedback, whose length changes according to the magnetic field intensity.</t>
+  </si>
+  <si>
+    <t>ADHD-Fueled Scattered Interests</t>
+  </si>
+  <si>
+    <t>Hakeem</t>
+  </si>
+  <si>
+    <t>An interesting dichotomy of absurdist humor and experimental voices, we bet you will LOL a lot or be like "damn this shit is good!" 
 Brought to you by TIMFL Studios</t>
   </si>
   <si>
-    <t>M.A.S/TIMFL Studios</t>
-  </si>
-  <si>
-    <t>Though MANIC is a solo endeavour, this compilation features many collaborations; namely with Dave Ewenson, Solomon Vroman, Yaya Wagg, Jeremy Costello and Camella Lobo. Adverse to drawing influence through genre; these sonic explorations are as poetic in ethos as they are in content. Recorded 2010-2015.</t>
-  </si>
-  <si>
-    <t>MANIC</t>
-  </si>
-  <si>
-    <t>the ancient ruins of modernity</t>
-  </si>
-  <si>
-    <t>“Relaxing sounds!! Light a candle, crack a cold alpine, and put on a sheet mask”</t>
-  </si>
-  <si>
-    <t>East Coast Lifestyle</t>
-  </si>
-  <si>
-    <t>Casiotone Demo Song compilation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Compilation including the sounds of Casio CA-100, CTK-450, CT-657, CT-700, EP-20, MT-240, PT-88, SK-5, SK-1, SA-1, SA-7, SA-75 and the VL-1. </t>
-  </si>
-  <si>
-    <t>Solarise</t>
-  </si>
-  <si>
-    <t>Martin Peach</t>
-  </si>
-  <si>
-    <t>This recording is made using a Pure Data patch that requests a file of solar wind measurements from the ACE satellite (http://www.srl.caltech.edu/ACE/) every two minutes. The North-South magnetic field intensity from the past two hours is played back over two minutes as notes in a 17-tone scale. The sound is Karplus-Strong string synthesis made to emulate a bowed instrument. The sound is then passed through a delay with feedback, whose length changes according to the magnetic field intensity.</t>
-  </si>
-  <si>
-    <t>Two 30-minute soundscapes by two babies from the Maritimes, trying to catch some relaxing vibes in the city</t>
+    <t xml:space="preserve">DIRTY STINKY SMELLY </t>
+  </si>
+  <si>
+    <t>PWUPPY PWINCESS</t>
+  </si>
+  <si>
+    <t>Casiotone demo song compilation</t>
+  </si>
+  <si>
+    <t>Juice it Up! // M.A.S</t>
+  </si>
+  <si>
+    <t>TIMFL Studios // SAGE aka victor</t>
+  </si>
+  <si>
+    <t>Boioioing!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You Look Fine </t>
+  </si>
+  <si>
+    <t>"Relaxing sounds!! Light a candle, crack a cold alpine, and put on a sheet mask"</t>
+  </si>
+  <si>
+    <t>Two 30-minute soundscapes by two babies from the Maritimes, trying to catch some relaxing vibes in the city.</t>
+  </si>
+  <si>
+    <t>A live performance exploring time and space with a variety of synthesizers.</t>
   </si>
 </sst>
 </file>
@@ -357,7 +355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -386,6 +384,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -700,10 +701,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{509B4220-E834-8A48-82FB-A9FB9AAA8E06}">
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -735,7 +736,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>8</v>
@@ -746,7 +747,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="1" t="s">
@@ -758,7 +759,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="1" t="s">
@@ -787,13 +788,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>12</v>
@@ -804,13 +805,13 @@
         <v>3</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>13</v>
@@ -821,13 +822,13 @@
         <v>3</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>60</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>14</v>
@@ -838,13 +839,13 @@
         <v>3</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>15</v>
@@ -858,7 +859,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>8</v>
@@ -869,7 +870,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="3" t="s">
@@ -881,7 +882,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="3" t="s">
@@ -910,13 +911,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>12</v>
@@ -927,30 +928,30 @@
         <v>4</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="136" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="31" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>55</v>
+        <v>61</v>
+      </c>
+      <c r="C17" t="s">
+        <v>35</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>14</v>
@@ -960,15 +961,9 @@
       <c r="A18" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>58</v>
-      </c>
+      <c r="B18" s="18"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
       <c r="E18" s="3" t="s">
         <v>15</v>
       </c>
@@ -981,7 +976,7 @@
         <v>5</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>8</v>
@@ -992,7 +987,7 @@
         <v>5</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="1" t="s">
@@ -1004,7 +999,7 @@
         <v>5</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="1" t="s">
@@ -1033,30 +1028,30 @@
         <v>5</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="C24" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="106" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="46" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>5</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>13</v>
@@ -1067,13 +1062,13 @@
         <v>5</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>66</v>
+        <v>23</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>14</v>
@@ -1083,14 +1078,14 @@
       <c r="A27" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>38</v>
+      <c r="B27" s="9" t="s">
+        <v>40</v>
       </c>
       <c r="C27" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="D27" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>15</v>
@@ -1104,7 +1099,7 @@
         <v>6</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>8</v>
@@ -1115,7 +1110,7 @@
         <v>6</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="3" t="s">
@@ -1127,7 +1122,7 @@
         <v>6</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="3" t="s">
@@ -1156,13 +1151,13 @@
         <v>6</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>12</v>
@@ -1173,13 +1168,13 @@
         <v>6</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>64</v>
+        <v>25</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>13</v>
@@ -1190,13 +1185,13 @@
         <v>6</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>14</v>
@@ -1207,13 +1202,13 @@
         <v>6</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>15</v>
@@ -1228,7 +1223,7 @@
         <v>7</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>8</v>
@@ -1239,7 +1234,7 @@
         <v>7</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="3" t="s">
@@ -1251,7 +1246,7 @@
         <v>7</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="3" t="s">
@@ -1279,48 +1274,48 @@
       <c r="A42" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>19</v>
+      <c r="B42" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C42" t="s">
+        <v>57</v>
+      </c>
+      <c r="D42" t="s">
+        <v>47</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D43" s="15" t="s">
-        <v>54</v>
+      <c r="B43" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C43" t="s">
+        <v>49</v>
+      </c>
+      <c r="D43" t="s">
+        <v>48</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" ht="106" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D44" s="14" t="s">
-        <v>32</v>
+        <v>26</v>
+      </c>
+      <c r="C44" t="s">
+        <v>27</v>
+      </c>
+      <c r="D44" s="20" t="s">
+        <v>45</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>14</v>
@@ -1331,12 +1326,12 @@
         <v>7</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D45" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D45" s="5" t="s">
         <v>68</v>
       </c>
       <c r="E45" s="3" t="s">
@@ -1348,6 +1343,51 @@
     </row>
     <row r="48" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="B48" s="19"/>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D50" s="7"/>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D51" s="13"/>
+    </row>
+    <row r="52" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D52" s="8"/>
+    </row>
+    <row r="55" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D55" s="7"/>
+    </row>
+    <row r="56" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D56" s="7"/>
+    </row>
+    <row r="57" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D57" s="7"/>
+    </row>
+    <row r="58" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D58" s="16"/>
+    </row>
+    <row r="59" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D59" s="17"/>
+    </row>
+    <row r="60" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D60" s="7"/>
+    </row>
+    <row r="61" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D61" s="15"/>
+    </row>
+    <row r="62" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D62" s="14"/>
+    </row>
+    <row r="63" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D63" s="8"/>
+    </row>
+    <row r="64" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D64" s="7"/>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D65" s="8"/>
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D66" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated schedule for week of feb 17th to 21st
</commit_message>
<xml_diff>
--- a/scheduleSheet/schedule.xlsx
+++ b/scheduleSheet/schedule.xlsx
@@ -1,39 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/SWOON1/Documents/GitHub/imca-raydeeoh/scheduleSheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/imcadepot2/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{345DC1FC-A68D-1543-BA93-A1FA40E8DC13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8035C9BB-EA00-E44F-BE2A-C20B81049307}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14160" xr2:uid="{C1F8DBFD-48D2-814D-8C9A-C834504E829D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="60">
   <si>
     <t>Day</t>
   </si>
@@ -212,6 +204,17 @@
   </si>
   <si>
     <t>b3tty.p</t>
+  </si>
+  <si>
+    <t>DYLAN JOSEPH CRICHTON 1978-2008 Beloved son, brother, and friend Dylan died peacefully in his sleep on June 10, 2008, 13 days before his 30th birthday. Dylan left in his wake many deeply affected and heartbroken family and friends, a large collection of lost cat posters and a wealth of unread thoughts, writings and music.
+Receiving his Bachelor of Fine Arts in 2002, Dylan only just prevented himself from taking legal action against what he called 'the system of accreditation'. Dylan's love of simple things cannot be adequately expressed in words, and memories of his particular distastes will always bring smiles to those who knew him well. He enjoyed playing piano, fundamentalist infomercials, gourmet cooking, tennis, the crepuscule, taking taxis, talking to strangers, white wine, summer rains, wearing his friends’ clothes, and girls. He disliked moths, other fluttering insects, girls, nitrates, and getting his picture taken.
+Dylan had a vast, of ten premonitory understanding of the world which he could make manifest in terrifying, satirical and beautiful ways. Though this sensibility sometimes clouded other aspects of life, he cared about the people close to him in a manner that transcended any concern for himself.</t>
+  </si>
+  <si>
+    <t>Now that the future is eminently expressive "but all the
+more obedient to simple sensory schemata", Betty P is finding
+immediate pleasure in a mediated present. Paradised, we’re all stuck
+here. And it’s getting hard to tell which fruit is the truth.</t>
   </si>
 </sst>
 </file>
@@ -330,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -361,6 +364,9 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -679,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{509B4220-E834-8A48-82FB-A9FB9AAA8E06}">
   <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
@@ -901,14 +907,14 @@
       <c r="A16" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>39</v>
+      <c r="B16" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>45</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>13</v>
@@ -980,7 +986,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="34">
+    <row r="23" spans="1:5" ht="306">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -990,8 +996,8 @@
       <c r="C23" t="s">
         <v>47</v>
       </c>
-      <c r="D23" s="6" t="s">
-        <v>21</v>
+      <c r="D23" s="22" t="s">
+        <v>58</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>11</v>
@@ -1035,14 +1041,14 @@
       <c r="A26" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>31</v>
+      <c r="B26" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>14</v>
@@ -1130,12 +1136,14 @@
       <c r="C33" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D33" s="7"/>
+      <c r="D33" s="7" t="s">
+        <v>31</v>
+      </c>
       <c r="E33" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" ht="61">
       <c r="A34" s="2" t="s">
         <v>6</v>
       </c>
@@ -1145,7 +1153,9 @@
       <c r="C34" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D34" s="8"/>
+      <c r="D34" s="16" t="s">
+        <v>59</v>
+      </c>
       <c r="E34" s="3" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
new schedule for replay week (feb)
</commit_message>
<xml_diff>
--- a/scheduleSheet/schedule.xlsx
+++ b/scheduleSheet/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/SWOON1/Documents/GitHub/imca-raydeeoh/scheduleSheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/imcadepot2/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{666F4C3D-B284-2940-B35D-DF67A60F6ED1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F033874-5DB2-C64E-ACBC-A6C4A7E881E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14140" xr2:uid="{C1F8DBFD-48D2-814D-8C9A-C834504E829D}"/>
+    <workbookView xWindow="400" yWindow="1040" windowWidth="25600" windowHeight="14160" xr2:uid="{C1F8DBFD-48D2-814D-8C9A-C834504E829D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="58">
   <si>
     <t>Day</t>
   </si>
@@ -174,12 +174,6 @@
   </si>
   <si>
     <t xml:space="preserve">Solarise </t>
-  </si>
-  <si>
-    <t>Juice it Up!</t>
-  </si>
-  <si>
-    <t>TIMFL studios</t>
   </si>
   <si>
     <t>DIRTY STINKY SMELLY</t>
@@ -209,6 +203,12 @@
   </si>
   <si>
     <t>THIS IS OUR TIMELAPSE</t>
+  </si>
+  <si>
+    <t>Juice it Up! // "She's too loud"</t>
+  </si>
+  <si>
+    <t>TIMFL studios // Sara-Claudia Ligondé</t>
   </si>
 </sst>
 </file>
@@ -218,7 +218,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -288,14 +288,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <i/>
-      <sz val="12"/>
-      <color rgb="FF222222"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="15"/>
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
@@ -327,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -356,7 +348,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -679,8 +670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{509B4220-E834-8A48-82FB-A9FB9AAA8E06}">
   <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
@@ -759,35 +750,35 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="85">
+    <row r="6" spans="1:5" ht="20">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>52</v>
+        <v>49</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="17">
+    <row r="7" spans="1:5" ht="46">
       <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
+      <c r="B7" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>39</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>13</v>
@@ -797,13 +788,15 @@
       <c r="A8" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>28</v>
+      <c r="B8" s="9" t="s">
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="7"/>
+        <v>30</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>42</v>
+      </c>
       <c r="E8" s="1" t="s">
         <v>14</v>
       </c>
@@ -884,31 +877,31 @@
       <c r="A15" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="12" t="s">
-        <v>47</v>
+      <c r="B15" s="9" t="s">
+        <v>48</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" ht="85">
       <c r="A16" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="9" t="s">
-        <v>29</v>
+      <c r="B16" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>42</v>
+        <v>24</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>50</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>13</v>
@@ -918,14 +911,14 @@
       <c r="A17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="9" t="s">
-        <v>29</v>
+      <c r="B17" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>42</v>
+        <v>28</v>
+      </c>
+      <c r="D17" t="s">
+        <v>28</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>14</v>
@@ -935,9 +928,15 @@
       <c r="A18" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
+      <c r="B18" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" t="s">
+        <v>28</v>
+      </c>
       <c r="E18" s="3" t="s">
         <v>15</v>
       </c>
@@ -990,59 +989,59 @@
       <c r="C23" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="22" t="s">
-        <v>54</v>
+      <c r="D23" s="21" t="s">
+        <v>52</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" ht="17">
       <c r="A24" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="9" t="s">
-        <v>41</v>
+      <c r="B24" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="C24" t="s">
-        <v>31</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>33</v>
+        <v>20</v>
+      </c>
+      <c r="D24" t="s">
+        <v>34</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="46">
+    <row r="25" spans="1:5" ht="17">
       <c r="A25" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>39</v>
+      <c r="B25" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" t="s">
+        <v>34</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" ht="61">
       <c r="A26" t="s">
         <v>5</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>36</v>
+        <v>55</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>53</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>14</v>
@@ -1120,52 +1119,52 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" ht="17">
       <c r="A33" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B33" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>56</v>
+      <c r="B33" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" t="s">
+        <v>46</v>
+      </c>
+      <c r="D33" t="s">
+        <v>22</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="61">
+    <row r="34" spans="1:5">
       <c r="A34" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B34" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D34" s="16" t="s">
-        <v>55</v>
+      <c r="B34" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="20">
+    <row r="35" spans="1:5">
       <c r="A35" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="C35" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>25</v>
+      <c r="B35" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>14</v>
@@ -1248,31 +1247,31 @@
       <c r="A42" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="10" t="s">
-        <v>32</v>
+      <c r="B42" s="9" t="s">
+        <v>41</v>
       </c>
       <c r="C42" t="s">
-        <v>20</v>
-      </c>
-      <c r="D42" t="s">
-        <v>34</v>
+        <v>31</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="17">
+    <row r="43" spans="1:5">
       <c r="A43" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C43" t="s">
-        <v>20</v>
-      </c>
-      <c r="D43" t="s">
-        <v>34</v>
+      <c r="B43" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>54</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>13</v>
@@ -1316,7 +1315,7 @@
       <c r="E46" s="1"/>
     </row>
     <row r="48" spans="1:5" ht="19">
-      <c r="B48" s="19"/>
+      <c r="B48" s="18"/>
     </row>
     <row r="50" spans="4:4">
       <c r="D50" s="7"/>

</xml_diff>